<commit_message>
finished movement and float text
</commit_message>
<xml_diff>
--- a/AutoChessServer/_Out/NFDataCfg/Excel/Comm/EffectData.xlsx
+++ b/AutoChessServer/_Out/NFDataCfg/Excel/Comm/EffectData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AutoChessServer\_Out\NFDataCfg\Excel\Comm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MyAutoChess\AutoChessServer\_Out\NFDataCfg\Excel\Comm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A43D97D-F34D-4549-83F4-32D9F9033A67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ED4C23-743B-47A9-9383-A037B5CCB124}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -915,7 +915,7 @@
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -995,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
@@ -1024,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -2256,10 +2256,10 @@
         <v>55</v>
       </c>
       <c r="B31">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C31">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2286,7 +2286,7 @@
         <v>25</v>
       </c>
       <c r="L31">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="M31">
         <v>1</v>
@@ -2300,10 +2300,10 @@
         <v>56</v>
       </c>
       <c r="B32">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -2330,7 +2330,7 @@
         <v>25</v>
       </c>
       <c r="L32">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="M32">
         <v>1</v>
@@ -2344,10 +2344,10 @@
         <v>57</v>
       </c>
       <c r="B33">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2374,7 +2374,7 @@
         <v>50</v>
       </c>
       <c r="L33">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="M33">
         <v>1</v>

</xml_diff>